<commit_message>
Se agregaron tres archivos
</commit_message>
<xml_diff>
--- a/Prueba_de_GIT.xlsx
+++ b/Prueba_de_GIT.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Hola</t>
+  </si>
+  <si>
+    <t>Otro</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -368,6 +371,11 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lunes 13 de Setiembre
</commit_message>
<xml_diff>
--- a/Prueba_de_GIT.xlsx
+++ b/Prueba_de_GIT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Hola</t>
   </si>
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,6 +386,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ültima actualiazción dom 19/9
</commit_message>
<xml_diff>
--- a/Prueba_de_GIT.xlsx
+++ b/Prueba_de_GIT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Hola</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>Algo mas</t>
+  </si>
+  <si>
+    <t>Seguimos</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A5"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,6 +394,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>